<commit_message>
Add new features and funcionality
</commit_message>
<xml_diff>
--- a/RESTFUL ROUTES.xlsx
+++ b/RESTFUL ROUTES.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>/home</t>
   </si>
   <si>
-    <t>/home/new</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>.findByIdAndRemove()</t>
+  </si>
+  <si>
+    <t>/new</t>
   </si>
 </sst>
 </file>
@@ -438,17 +438,17 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="1" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,10 +462,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -473,33 +473,33 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -507,81 +507,81 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>